<commit_message>
updated grade spreadsheet for PHY410
</commit_message>
<xml_diff>
--- a/PHY410/grade.xlsx
+++ b/PHY410/grade.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crispda1\Documents\git\SPRING2018\PHY410\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crispda1\Documents\SPRING2018\PHY410\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -383,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,10 +413,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1">
-        <f>B5/C5</f>
+        <f t="shared" ref="E5:E15" si="0">B5/C5</f>
         <v>0</v>
       </c>
     </row>
@@ -428,10 +428,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1">
-        <f>B6/C6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -443,10 +443,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1">
-        <f>B7/C7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -455,14 +455,14 @@
         <v>4</v>
       </c>
       <c r="B8" s="2">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1">
-        <f>B8/C8</f>
-        <v>0.85</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -470,14 +470,14 @@
         <v>5</v>
       </c>
       <c r="B9" s="2">
-        <v>8.5</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1">
-        <f>B9/C9</f>
-        <v>0.85</v>
+        <f t="shared" si="0"/>
+        <v>0.93333333333333335</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -485,14 +485,14 @@
         <v>6</v>
       </c>
       <c r="B10" s="2">
-        <v>8.5</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1">
-        <f>B10/C10</f>
-        <v>0.85</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -500,14 +500,14 @@
         <v>7</v>
       </c>
       <c r="B11" s="2">
-        <v>8.5</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1">
-        <f>B11/C11</f>
-        <v>0.85</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -515,14 +515,14 @@
         <v>8</v>
       </c>
       <c r="B12" s="2">
-        <v>8.5</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1">
-        <f>B12/C12</f>
-        <v>0.85</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -530,14 +530,14 @@
         <v>9</v>
       </c>
       <c r="B13" s="2">
-        <v>8.5</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E13" s="1">
-        <f>B13/C13</f>
-        <v>0.85</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -545,14 +545,14 @@
         <v>10</v>
       </c>
       <c r="B14" s="2">
-        <v>8.5</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1">
-        <f>B14/C14</f>
-        <v>0.85</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -560,14 +560,14 @@
         <v>11</v>
       </c>
       <c r="B15" s="2">
-        <v>8.5</v>
+        <v>15</v>
       </c>
       <c r="C15" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E15" s="1">
-        <f>B15/C15</f>
-        <v>0.85</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
       </c>
       <c r="E17" s="1">
         <f>AVERAGE(E5:E15)</f>
-        <v>0.61818181818181805</v>
+        <v>0.68484848484848482</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
       </c>
       <c r="E18">
         <f>E17*E3</f>
-        <v>12.363636363636362</v>
+        <v>13.696969696969695</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -611,14 +611,14 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="C23">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E23" s="1">
         <f>B23/C23</f>
-        <v>0.85</v>
+        <v>0.68333333333333335</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,14 +626,14 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="C24">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" ref="E24:E25" si="0">B24/C24</f>
-        <v>0.85</v>
+        <f t="shared" ref="E24:E25" si="1">B24/C24</f>
+        <v>0.73333333333333328</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -641,14 +641,14 @@
         <v>3</v>
       </c>
       <c r="B25">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C25">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="0"/>
-        <v>0.85</v>
+        <f t="shared" si="1"/>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
       </c>
       <c r="E27" s="1">
         <f>AVERAGE(E23:E25)</f>
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
       </c>
       <c r="E28">
         <f>E27*E21</f>
-        <v>38.25</v>
+        <v>33.75</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -689,14 +689,14 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C33">
         <v>100</v>
       </c>
       <c r="E33" s="1">
         <f>B33/C33</f>
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
       </c>
       <c r="E35">
         <f>E33*E31</f>
-        <v>29.75</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
       </c>
       <c r="E37">
         <f>E18+E28+E35</f>
-        <v>80.36363636363636</v>
+        <v>75.446969696969688</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,7 +726,7 @@
       </c>
       <c r="E38" s="1">
         <f>E37*0.01</f>
-        <v>0.80363636363636359</v>
+        <v>0.7544696969696969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>